<commit_message>
restructured code and added sorting:   main.py
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C10"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,156 +421,275 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Item name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Shop</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GeForce RTX 3070 Extreme Gaming 8GB GDDR6 256bit Biostar</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>457.00 €</t>
-        </is>
+          <t>GeForce RTX 3060 Ventus 2X OC 12GB GDDR6 192bit MSI</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>290</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GeForce RTX 3070 8GB GDDR6 256bit Biostar</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>471.00 €</t>
-        </is>
+          <t>GeForce RTX 3060 Gaming OC 8GB GDDR6 128bit rev. 2.0 Gigabyte</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>292</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GeForce RTX 3070 Gaming Twin Edge LHR 8GB GDDR6 256bit ZOTAC</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>690.99 €</t>
-        </is>
+          <t>GeForce RTX 3060 Gaming OC 8GB GDDR6 128bit Gigabyte</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>292.63</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GeForce RTX 3070 Ti GameRock 8GB GDDR6X 256bit Palit</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>928.99 €</t>
-        </is>
+          <t>GeForce RTX 3060 WindForce OC 12GB GDDR6 192bit Gigabyte</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>300.18</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EK-Quantum Vector FTW3 RTX 3070 D-RGB EKWB</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>154.99 €</t>
-        </is>
+          <t>GeForce RTX 3060 Gaming OC 12GB GDDR6 192bit rev. 2.0 LHR Gigabyte</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>302.99</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Water Blocks Quantum Vector FE RTX 3070 Backplate EKWB</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>34.99 €</t>
-        </is>
+          <t>GeForce RTX 3060 Dual OC V2 LHR 12GB GDDR6 192bit Asus</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>317.9</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EK-Quantum Vector GeForce FTW3 RTX 3070 D-RGB Water Block EKWB</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>152.99 €</t>
-        </is>
+          <t>GeForce RTX Extreme Gaming 3060 12GB GDDR6 192bit Biostar</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>317.9</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16" Omen 16-c0086nf Ryzen 7 5800H 16GB 512GB SSD RTX 3070 W11 Renew HP</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1242.99 €</t>
-        </is>
+          <t>GeForce RTX 3060 V2 OC 12GB GDDR6 192bit Asus</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>329</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Legion 5 15ACH6H 15.6 165hz 5600H 16GB 1SSD RTX3070 EN DOS 82JU00JQPB Lenovo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1366.07 €</t>
-        </is>
+          <t>GeForce RTX 3060 Twin Twin Edge 12GB GDDR6 192bit ZOTAC</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>334.98</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RD</t>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>GeForce RTX 3060 Twin X2 OC LHR 12GB GDDR6 192bit Inno3D</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>341</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GeForce RTX 3060 Twin X2 12GB GDDR6 192bit Inno3D</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>351</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>GeForce RTX 3060 Ti Extreme Gaming 8GB GDDR6X 256bit Biostar</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>361</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5500 16GB 250SSD RTX3060 12GB no-OS INTOP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>699.99</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5500 16GB 500SSD RTX3060 12GB no-OS INTOP</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>711.99</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5500 32GB 250SSD RTX3060 12GB no-OS INTOP</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>728.99</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ryzen 5 5600X 16GB 250SSD RTX3060 12GB no-OS INTOP</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>734.99</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Blade RZ09-0421EED3-R3E1 15.6 240hz i7-12800H 16GB 1SSD RTX3060 EN W11 Razer</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3340</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>RD Electronics</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   data.xlsx 	modified:   main.py
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,71 +441,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Ventus 2X OC 12GB GDDR6 192bit MSI</t>
+          <t>Xiaomi Redmi Watch 5 Active, matte silver - Smartwatch</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>290</v>
+        <v>39.99</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Gaming OC 8GB GDDR6 128bit rev. 2.0 Gigabyte</t>
+          <t>Xiaomi Redmi Buds 5, black - Wireless earbuds</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>292</v>
+        <v>39.99</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Gaming OC 8GB GDDR6 128bit Gigabyte</t>
+          <t>Xiaomi Redmi Watch 5 Lite, black - Smartwatch</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>292.63</v>
+        <v>49.99</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 WindForce OC 12GB GDDR6 192bit Gigabyte</t>
+          <t>Xiaomi Redmi Watch 5 Lite, light gold - Smartwatch</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>300.18</v>
+        <v>49.99</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Gaming OC 12GB GDDR6 192bit rev. 2.0 LHR Gigabyte</t>
+          <t>Redmi A5 3/ 64GB Lake Green Xiaomi</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>302.99</v>
+        <v>76.98999999999999</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -516,11 +516,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Dual OC V2 LHR 12GB GDDR6 192bit Asus</t>
+          <t>Redmi A5 3/ 64GB Midnight Black Xiaomi</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>317.9</v>
+        <v>79</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -531,11 +531,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GeForce RTX Extreme Gaming 3060 12GB GDDR6 192bit Biostar</t>
+          <t>Redmi A5 3/ 64GB Sandy Gold Xiaomi</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>317.9</v>
+        <v>79</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -546,11 +546,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 V2 OC 12GB GDDR6 192bit Asus</t>
+          <t>Redmi A5 3/ 64GB Ocean Blue Xiaomi</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>329</v>
+        <v>79</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -561,11 +561,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Twin Twin Edge 12GB GDDR6 192bit ZOTAC</t>
+          <t>Redmi A5 4/ 128GB Ocean Blue Xiaomi</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>334.98</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -576,11 +576,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Twin X2 OC LHR 12GB GDDR6 192bit Inno3D</t>
+          <t>Redmi A5 4/ 128GB Lake Green Xiaomi</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>341</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -591,11 +591,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Twin X2 12GB GDDR6 192bit Inno3D</t>
+          <t>Redmi A5 4/ 128GB Midnight Black Xiaomi</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>351</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -606,90 +606,285 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GeForce RTX 3060 Ti Extreme Gaming 8GB GDDR6X 256bit Biostar</t>
+          <t>Xiaomi Redmi Watch 5, purple - Smartwatch</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>361</v>
+        <v>109.99</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ryzen 5 5500 16GB 250SSD RTX3060 12GB no-OS INTOP</t>
+          <t>Xiaomi Redmi Watch 5, black - Smartwatch</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>699.99</v>
+        <v>109.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ryzen 5 5500 16GB 500SSD RTX3060 12GB no-OS INTOP</t>
+          <t>Xiaomi Redmi A5, midnight black - Smartphone</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>711.99</v>
+        <v>109.99</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ryzen 5 5500 32GB 250SSD RTX3060 12GB no-OS INTOP</t>
+          <t>Xiaomi Redmi A5, sandy gold - Smartphone</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>728.99</v>
+        <v>109.99</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ryzen 5 5600X 16GB 250SSD RTX3060 12GB no-OS INTOP</t>
+          <t>Xiaomi Redmi Watch 5, silver - Smartwatch</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>734.99</v>
+        <v>109.99</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>RD Electronics</t>
+          <t>Euronics</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Blade RZ09-0421EED3-R3E1 15.6 240hz i7-12800H 16GB 1SSD RTX3060 EN W11 Razer</t>
+          <t>Xiaomi Redmi A5, ocean blue - Smartphone</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3340</v>
+        <v>109.99</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Redmi A5 4/ 128GB Sandy Gold Xiaomi</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>124.99</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>RD Electronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 12 5G, 128 GB, green - Smartphone</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>179.99</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 13 5G, 256 GB, blue - Smartphone</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>219.99</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 5G, 6 GB, 128 GB, midnight black - Smartphone</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>229.99</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 5G, 6 GB, 128 GB, coral green - Smartphone</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>229.99</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 5G, 8 GB, 256 GB, coral green - Smartphone</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>249.99</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 5G, 8 GB, 256 GB, midnight black - Smartphone</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>249.99</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro 5G, lavender purple - Smartphone</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>299.99</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro 5G, coral green - Smartphone</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>299.99</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro 5G, midnight black - Smartphone</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>299.99</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro+ 5G, frost blue - Smartphone</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>399.99</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro+ 5G, midnight black - Smartphone</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>399.99</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Euronics</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 14 Pro+ 5G, lavender purple - Smartphone</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>399.99</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Euronics</t>
         </is>
       </c>
     </row>

</xml_diff>